<commit_message>
Add comments && Update functions and variables
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBB1825-D4F0-4C50-943C-25153C45726B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E60DBE3-C9BA-459D-AB64-0229FE9AA979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,7 +373,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>